<commit_message>
modified to work on Mac
</commit_message>
<xml_diff>
--- a/data/complete_data.xlsx
+++ b/data/complete_data.xlsx
@@ -3604,7 +3604,7 @@
         <v>42.360095</v>
       </c>
       <c r="M4">
-        <v>-71.09211500000001</v>
+        <v>-71.092115</v>
       </c>
       <c r="N4" t="s">
         <v>634</v>
@@ -3819,7 +3819,7 @@
         <v>635</v>
       </c>
       <c r="O5">
-        <v>0.06950000000000001</v>
+        <v>0.0695</v>
       </c>
       <c r="P5">
         <v>0.0694937361604</v>
@@ -4434,13 +4434,13 @@
         <v>40.34853</v>
       </c>
       <c r="M8">
-        <v>-74.66360299999999</v>
+        <v>-74.663603</v>
       </c>
       <c r="N8" t="s">
         <v>638</v>
       </c>
       <c r="O8">
-        <v>0.07439999999999999</v>
+        <v>0.0744</v>
       </c>
       <c r="P8">
         <v>0.0744341428625</v>
@@ -4930,7 +4930,7 @@
         <v>127400</v>
       </c>
       <c r="AV10">
-        <v>0.008200000000000001</v>
+        <v>0.0082</v>
       </c>
       <c r="AW10">
         <v>29</v>
@@ -5034,7 +5034,7 @@
         <v>42.447199</v>
       </c>
       <c r="M11">
-        <v>-76.48348900000001</v>
+        <v>-76.483489</v>
       </c>
       <c r="N11" t="s">
         <v>641</v>
@@ -5640,7 +5640,7 @@
         <v>39.32838</v>
       </c>
       <c r="M14">
-        <v>-76.62079900000001</v>
+        <v>-76.620799</v>
       </c>
       <c r="N14" t="s">
         <v>644</v>
@@ -7121,7 +7121,7 @@
         <v>101900</v>
       </c>
       <c r="AV21">
-        <v>0.09959999999999999</v>
+        <v>0.0996</v>
       </c>
       <c r="AW21">
         <v>73</v>
@@ -7643,7 +7643,7 @@
         <v>40.108864</v>
       </c>
       <c r="M24">
-        <v>-88.23030900000001</v>
+        <v>-88.230309</v>
       </c>
       <c r="N24" t="s">
         <v>654</v>
@@ -7852,7 +7852,7 @@
         <v>35.912165</v>
       </c>
       <c r="M25">
-        <v>-79.05096899999999</v>
+        <v>-79.050969</v>
       </c>
       <c r="N25" t="s">
         <v>655</v>
@@ -8061,7 +8061,7 @@
         <v>38.037796</v>
       </c>
       <c r="M26">
-        <v>-78.50515300000001</v>
+        <v>-78.505153</v>
       </c>
       <c r="N26" t="s">
         <v>656</v>
@@ -8270,7 +8270,7 @@
         <v>40.503796</v>
       </c>
       <c r="M27">
-        <v>-74.45050999999999</v>
+        <v>-74.45051</v>
       </c>
       <c r="N27" t="s">
         <v>657</v>
@@ -8658,7 +8658,7 @@
         <v>44.977886</v>
       </c>
       <c r="M29">
-        <v>-93.23535200000001</v>
+        <v>-93.235352</v>
       </c>
       <c r="N29" t="s">
         <v>659</v>
@@ -9076,7 +9076,7 @@
         <v>40.444502</v>
       </c>
       <c r="M31">
-        <v>-79.95469199999999</v>
+        <v>-79.954692</v>
       </c>
       <c r="N31" t="s">
         <v>661</v>
@@ -11629,7 +11629,7 @@
         <v>96700</v>
       </c>
       <c r="AV43">
-        <v>0.07340000000000001</v>
+        <v>0.0734</v>
       </c>
       <c r="AW43">
         <v>142</v>
@@ -11942,7 +11942,7 @@
         <v>43.126437</v>
       </c>
       <c r="M45">
-        <v>-77.63104199999999</v>
+        <v>-77.631042</v>
       </c>
       <c r="N45" t="s">
         <v>675</v>
@@ -12968,7 +12968,7 @@
         <v>681</v>
       </c>
       <c r="O51">
-        <v>0.08740000000000001</v>
+        <v>0.0874</v>
       </c>
       <c r="P51">
         <v>0.08744372514869</v>
@@ -13374,7 +13374,7 @@
         <v>41.703058</v>
       </c>
       <c r="M53">
-        <v>-86.23895899999999</v>
+        <v>-86.238959</v>
       </c>
       <c r="N53" t="s">
         <v>683</v>
@@ -13461,7 +13461,7 @@
         <v>138000</v>
       </c>
       <c r="AV53">
-        <v>0.0005999999999999999</v>
+        <v>0.0006</v>
       </c>
       <c r="AW53">
         <v>49</v>
@@ -14589,7 +14589,7 @@
         <v>29.716485</v>
       </c>
       <c r="M59">
-        <v>-95.40362500000001</v>
+        <v>-95.403625</v>
       </c>
       <c r="N59" t="s">
         <v>689</v>
@@ -15440,7 +15440,7 @@
         <v>87100</v>
       </c>
       <c r="AV63">
-        <v>0.08550000000000001</v>
+        <v>0.0855</v>
       </c>
       <c r="AW63">
         <v>91</v>
@@ -15750,7 +15750,7 @@
         <v>32.845254</v>
       </c>
       <c r="M65">
-        <v>-96.78485499999999</v>
+        <v>-96.784855</v>
       </c>
       <c r="N65" t="s">
         <v>695</v>
@@ -16087,7 +16087,7 @@
         <v>33.50223</v>
       </c>
       <c r="M67">
-        <v>-86.80916999999999</v>
+        <v>-86.80917</v>
       </c>
       <c r="N67" t="s">
         <v>697</v>
@@ -16708,7 +16708,7 @@
         <v>40.913138</v>
       </c>
       <c r="M70">
-        <v>-73.12359499999999</v>
+        <v>-73.123595</v>
       </c>
       <c r="N70" t="s">
         <v>700</v>
@@ -17242,7 +17242,7 @@
         <v>703</v>
       </c>
       <c r="O73">
-        <v>0.8179999999999999</v>
+        <v>0.818</v>
       </c>
       <c r="P73">
         <v>0.81796829125073</v>
@@ -19570,7 +19570,7 @@
         <v>0.9142</v>
       </c>
       <c r="P85">
-        <v>0.9141878607217599</v>
+        <v>0.91418786072176</v>
       </c>
       <c r="W85">
         <v>22</v>
@@ -19854,7 +19854,7 @@
         <v>118600</v>
       </c>
       <c r="AV86">
-        <v>0.07829999999999999</v>
+        <v>0.0783</v>
       </c>
       <c r="AW86">
         <v>48</v>
@@ -19958,7 +19958,7 @@
         <v>42.386162</v>
       </c>
       <c r="M87">
-        <v>-72.52616999999999</v>
+        <v>-72.52617</v>
       </c>
       <c r="N87" t="s">
         <v>717</v>
@@ -20045,7 +20045,7 @@
         <v>80700</v>
       </c>
       <c r="AV87">
-        <v>0.08110000000000001</v>
+        <v>0.0811</v>
       </c>
       <c r="AW87">
         <v>44</v>
@@ -20155,7 +20155,7 @@
         <v>718</v>
       </c>
       <c r="O88">
-        <v>0.7766999999999999</v>
+        <v>0.7767</v>
       </c>
       <c r="P88">
         <v>0.77668572508623</v>
@@ -20355,7 +20355,7 @@
         <v>35.785111</v>
       </c>
       <c r="M89">
-        <v>-78.67451699999999</v>
+        <v>-78.674517</v>
       </c>
       <c r="N89" t="s">
         <v>719</v>
@@ -21325,7 +21325,7 @@
         <v>29.719988</v>
       </c>
       <c r="M94">
-        <v>-95.34485100000001</v>
+        <v>-95.344851</v>
       </c>
       <c r="N94" t="s">
         <v>723</v>
@@ -21686,7 +21686,7 @@
         <v>35.955093</v>
       </c>
       <c r="M96">
-        <v>-83.92969600000001</v>
+        <v>-83.929696</v>
       </c>
       <c r="N96" t="s">
         <v>725</v>
@@ -22101,13 +22101,13 @@
         <v>30.4421</v>
       </c>
       <c r="M98">
-        <v>-84.29480100000001</v>
+        <v>-84.294801</v>
       </c>
       <c r="N98" t="s">
         <v>727</v>
       </c>
       <c r="O98">
-        <v>0.5538999999999999</v>
+        <v>0.5539</v>
       </c>
       <c r="P98">
         <v>0.55385581180202</v>
@@ -22188,7 +22188,7 @@
         <v>76300</v>
       </c>
       <c r="AV98">
-        <v>0.06809999999999999</v>
+        <v>0.0681</v>
       </c>
       <c r="AW98">
         <v>92</v>
@@ -22298,10 +22298,10 @@
         <v>728</v>
       </c>
       <c r="O99">
-        <v>0.7534999999999999</v>
+        <v>0.7535</v>
       </c>
       <c r="P99">
-        <v>0.7534525367059099</v>
+        <v>0.75345253670591</v>
       </c>
       <c r="Q99">
         <v>500</v>
@@ -22498,13 +22498,13 @@
         <v>37.228572</v>
       </c>
       <c r="M100">
-        <v>-80.42322900000001</v>
+        <v>-80.423229</v>
       </c>
       <c r="N100" t="s">
         <v>729</v>
       </c>
       <c r="O100">
-        <v>0.7262999999999999</v>
+        <v>0.7263</v>
       </c>
       <c r="P100">
         <v>0.72633050520632</v>
@@ -22680,7 +22680,7 @@
         <v>35.208152</v>
       </c>
       <c r="M101">
-        <v>-97.44569199999999</v>
+        <v>-97.445692</v>
       </c>
       <c r="N101" t="s">
         <v>730</v>
@@ -23307,7 +23307,7 @@
         <v>733</v>
       </c>
       <c r="O104">
-        <v>0.5780999999999999</v>
+        <v>0.5781</v>
       </c>
       <c r="P104">
         <v>0.57806166318634</v>
@@ -23647,7 +23647,7 @@
         <v>42.339992</v>
       </c>
       <c r="M106">
-        <v>-71.08878199999999</v>
+        <v>-71.088782</v>
       </c>
       <c r="N106" t="s">
         <v>735</v>
@@ -24059,7 +24059,7 @@
         <v>40.607158</v>
       </c>
       <c r="M108">
-        <v>-75.37888700000001</v>
+        <v>-75.378887</v>
       </c>
       <c r="N108" t="s">
         <v>737</v>
@@ -24662,7 +24662,7 @@
         <v>42.728983</v>
       </c>
       <c r="M111">
-        <v>-73.67876800000001</v>
+        <v>-73.678768</v>
       </c>
       <c r="N111" t="s">
         <v>740</v>
@@ -25253,7 +25253,7 @@
         <v>40.819794</v>
       </c>
       <c r="M114">
-        <v>-73.95055000000001</v>
+        <v>-73.95055</v>
       </c>
       <c r="N114" t="s">
         <v>743</v>
@@ -25590,7 +25590,7 @@
         <v>43.044108</v>
       </c>
       <c r="M116">
-        <v>-88.02269800000001</v>
+        <v>-88.022698</v>
       </c>
       <c r="N116" t="s">
         <v>745</v>
@@ -25724,7 +25724,7 @@
         <v>40.822272</v>
       </c>
       <c r="M117">
-        <v>-96.70217700000001</v>
+        <v>-96.702177</v>
       </c>
       <c r="N117" t="s">
         <v>746</v>
@@ -25936,7 +25936,7 @@
         <v>747</v>
       </c>
       <c r="O118">
-        <v>0.7344000000000001</v>
+        <v>0.7344</v>
       </c>
       <c r="P118">
         <v>0.73441175256881</v>
@@ -26139,7 +26139,7 @@
         <v>41.874911</v>
       </c>
       <c r="M119">
-        <v>-87.66749799999999</v>
+        <v>-87.667498</v>
       </c>
       <c r="N119" t="s">
         <v>748</v>
@@ -27336,7 +27336,7 @@
         <v>39.188616</v>
       </c>
       <c r="M125">
-        <v>-96.58107699999999</v>
+        <v>-96.581077</v>
       </c>
       <c r="N125" t="s">
         <v>754</v>
@@ -27500,7 +27500,7 @@
         <v>29.311333</v>
       </c>
       <c r="M126">
-        <v>-94.77640100000001</v>
+        <v>-94.776401</v>
       </c>
       <c r="N126" t="s">
         <v>755</v>
@@ -28652,7 +28652,7 @@
         <v>28.60106</v>
       </c>
       <c r="M132">
-        <v>-81.19880499999999</v>
+        <v>-81.198805</v>
       </c>
       <c r="N132" t="s">
         <v>761</v>
@@ -28852,7 +28852,7 @@
         <v>0.6665</v>
       </c>
       <c r="P133">
-        <v>0.6664743475945299</v>
+        <v>0.66647434759453</v>
       </c>
       <c r="Q133">
         <v>520</v>
@@ -29652,7 +29652,7 @@
         <v>34.749718</v>
       </c>
       <c r="M137">
-        <v>-92.32094499999999</v>
+        <v>-92.320945</v>
       </c>
       <c r="N137" t="s">
         <v>766</v>
@@ -30377,7 +30377,7 @@
         <v>32.989432</v>
       </c>
       <c r="M141">
-        <v>-96.74837100000001</v>
+        <v>-96.748371</v>
       </c>
       <c r="N141" t="s">
         <v>770</v>
@@ -31210,7 +31210,7 @@
         <v>774</v>
       </c>
       <c r="O145">
-        <v>0.7495000000000001</v>
+        <v>0.7495</v>
       </c>
       <c r="P145">
         <v>0.74949017048698</v>
@@ -31956,7 +31956,7 @@
         <v>39.73686</v>
       </c>
       <c r="M149">
-        <v>-84.17366199999999</v>
+        <v>-84.173662</v>
       </c>
       <c r="N149" s="2" t="s">
         <v>778</v>
@@ -31965,7 +31965,7 @@
         <v>0.5901</v>
       </c>
       <c r="P149">
-        <v>0.5901272384542799</v>
+        <v>0.59012723845428</v>
       </c>
       <c r="Q149">
         <v>510</v>
@@ -32162,7 +32162,7 @@
         <v>39.326799</v>
       </c>
       <c r="M150">
-        <v>-82.10106399999999</v>
+        <v>-82.101064</v>
       </c>
       <c r="N150" t="s">
         <v>779</v>
@@ -32577,7 +32577,7 @@
         <v>41.833801</v>
       </c>
       <c r="M152">
-        <v>-87.62834599999999</v>
+        <v>-87.628346</v>
       </c>
       <c r="N152" t="s">
         <v>781</v>
@@ -33189,7 +33189,7 @@
         <v>0.8388</v>
       </c>
       <c r="P155">
-        <v>0.8387681159420201</v>
+        <v>0.83876811594202</v>
       </c>
       <c r="Q155">
         <v>480</v>
@@ -34404,7 +34404,7 @@
         <v>0.7267</v>
       </c>
       <c r="P161">
-        <v>0.7267206477732699</v>
+        <v>0.72672064777327</v>
       </c>
       <c r="Q161">
         <v>520</v>
@@ -34610,7 +34610,7 @@
         <v>791</v>
       </c>
       <c r="O162">
-        <v>0.6425999999999999</v>
+        <v>0.6426</v>
       </c>
       <c r="P162">
         <v>0.64260768335273</v>
@@ -35526,7 +35526,7 @@
         <v>0.8438</v>
       </c>
       <c r="P167">
-        <v>0.8438449612403101</v>
+        <v>0.84384496124031</v>
       </c>
       <c r="Q167">
         <v>470</v>
@@ -36514,7 +36514,7 @@
         <v>801</v>
       </c>
       <c r="O172">
-        <v>0.9782999999999999</v>
+        <v>0.9783</v>
       </c>
       <c r="P172">
         <v>0.97834047526295</v>
@@ -37010,7 +37010,7 @@
         <v>84200</v>
       </c>
       <c r="AV174">
-        <v>0.08649999999999999</v>
+        <v>0.0865</v>
       </c>
       <c r="AW174">
         <v>28</v>
@@ -37332,7 +37332,7 @@
         <v>0.5278</v>
       </c>
       <c r="P176">
-        <v>0.5277819083023499</v>
+        <v>0.52778190830235</v>
       </c>
       <c r="Q176">
         <v>500</v>
@@ -37532,7 +37532,7 @@
         <v>37.713239</v>
       </c>
       <c r="M177">
-        <v>-89.21872399999999</v>
+        <v>-89.218724</v>
       </c>
       <c r="N177" t="s">
         <v>806</v>
@@ -37744,7 +37744,7 @@
         <v>807</v>
       </c>
       <c r="O178">
-        <v>0.7102000000000001</v>
+        <v>0.7102</v>
       </c>
       <c r="P178">
         <v>0.71019877391788</v>
@@ -39395,7 +39395,7 @@
         <v>71700</v>
       </c>
       <c r="AV186">
-        <v>0.09909999999999999</v>
+        <v>0.0991</v>
       </c>
       <c r="AW186">
         <v>30</v>
@@ -39499,7 +39499,7 @@
         <v>42.653178</v>
       </c>
       <c r="M187">
-        <v>-73.77397499999999</v>
+        <v>-73.773975</v>
       </c>
       <c r="N187" t="s">
         <v>816</v>
@@ -39621,7 +39621,7 @@
         <v>32.525518</v>
       </c>
       <c r="M188">
-        <v>-92.64964000000001</v>
+        <v>-92.64964</v>
       </c>
       <c r="N188" t="s">
         <v>817</v>
@@ -39827,7 +39827,7 @@
         <v>40.741997</v>
       </c>
       <c r="M189">
-        <v>-74.17711300000001</v>
+        <v>-74.177113</v>
       </c>
       <c r="N189" t="s">
         <v>818</v>
@@ -39836,7 +39836,7 @@
         <v>0.6339</v>
       </c>
       <c r="P189">
-        <v>0.6338706301025701</v>
+        <v>0.63387063010257</v>
       </c>
       <c r="Q189">
         <v>490</v>
@@ -40248,7 +40248,7 @@
         <v>0.7591</v>
       </c>
       <c r="P191">
-        <v>0.7591240875912399</v>
+        <v>0.75912408759124</v>
       </c>
       <c r="Q191">
         <v>450</v>
@@ -40448,7 +40448,7 @@
         <v>43.090325</v>
       </c>
       <c r="M192">
-        <v>-77.67521000000001</v>
+        <v>-77.67521</v>
       </c>
       <c r="N192" t="s">
         <v>821</v>
@@ -41197,7 +41197,7 @@
         <v>37.955853</v>
       </c>
       <c r="M196">
-        <v>-91.77589999999999</v>
+        <v>-91.7759</v>
       </c>
       <c r="N196" t="s">
         <v>825</v>
@@ -41299,7 +41299,7 @@
         <v>95200</v>
       </c>
       <c r="AV196">
-        <v>0.06900000000000001</v>
+        <v>0.069</v>
       </c>
       <c r="AW196">
         <v>16</v>
@@ -41618,7 +41618,7 @@
         <v>0.8274</v>
       </c>
       <c r="P198">
-        <v>0.8274111675126899</v>
+        <v>0.82741116751269</v>
       </c>
       <c r="Q198">
         <v>475</v>
@@ -42227,7 +42227,7 @@
         <v>35.606347</v>
       </c>
       <c r="M201">
-        <v>-77.36619899999999</v>
+        <v>-77.366199</v>
       </c>
       <c r="N201" t="s">
         <v>830</v>
@@ -42645,7 +42645,7 @@
         <v>35.306834</v>
       </c>
       <c r="M203">
-        <v>-80.73578999999999</v>
+        <v>-80.73579</v>
       </c>
       <c r="N203" t="s">
         <v>832</v>
@@ -43269,7 +43269,7 @@
         <v>38.920739</v>
       </c>
       <c r="M206">
-        <v>-77.01947800000001</v>
+        <v>-77.019478</v>
       </c>
       <c r="N206" t="s">
         <v>835</v>
@@ -43371,7 +43371,7 @@
         <v>83600</v>
       </c>
       <c r="AV206">
-        <v>0.08599999999999999</v>
+        <v>0.086</v>
       </c>
       <c r="AW206">
         <v>35</v>
@@ -44012,7 +44012,7 @@
         <v>0.7077</v>
       </c>
       <c r="P210">
-        <v>0.7077268962252899</v>
+        <v>0.70772689622529</v>
       </c>
       <c r="Q210">
         <v>460</v>
@@ -44785,7 +44785,7 @@
         <v>31.327499</v>
       </c>
       <c r="M214">
-        <v>-89.33790999999999</v>
+        <v>-89.33791</v>
       </c>
       <c r="N214" t="s">
         <v>843</v>
@@ -44794,7 +44794,7 @@
         <v>0.6674</v>
       </c>
       <c r="P214">
-        <v>0.6673504273504201</v>
+        <v>0.66735042735042</v>
       </c>
       <c r="Q214">
         <v>450</v>
@@ -44991,7 +44991,7 @@
         <v>44.663761</v>
       </c>
       <c r="M215">
-        <v>-74.99994700000001</v>
+        <v>-74.999947</v>
       </c>
       <c r="N215" t="s">
         <v>844</v>
@@ -45000,7 +45000,7 @@
         <v>0.6214</v>
       </c>
       <c r="P215">
-        <v>0.6214025131738899</v>
+        <v>0.62140251317389</v>
       </c>
       <c r="Q215">
         <v>520</v>
@@ -45197,7 +45197,7 @@
         <v>47.919774</v>
       </c>
       <c r="M216">
-        <v>-97.07345100000001</v>
+        <v>-97.073451</v>
       </c>
       <c r="N216" t="s">
         <v>845</v>
@@ -45403,7 +45403,7 @@
         <v>38.935796</v>
       </c>
       <c r="M217">
-        <v>-76.99896099999999</v>
+        <v>-76.998961</v>
       </c>
       <c r="N217" t="s">
         <v>846</v>

</xml_diff>